<commit_message>
edits to resp rate data
</commit_message>
<xml_diff>
--- a/RAnalysis/Output/Water_Chemistry/MS_Table.xlsx
+++ b/RAnalysis/Output/Water_Chemistry/MS_Table.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3528" yWindow="0" windowWidth="20376" windowHeight="7212"/>
+    <workbookView xWindow="5880" yWindow="0" windowWidth="20376" windowHeight="7212"/>
   </bookViews>
   <sheets>
     <sheet name="SummaryTable_meanSE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -197,54 +197,30 @@
     <t>7.69 ± 0.007</t>
   </si>
   <si>
-    <t>1770 ± 7.18</t>
-  </si>
-  <si>
     <t>1840 ± 8.18</t>
   </si>
   <si>
     <t>7.67 ± 0.008</t>
   </si>
   <si>
-    <t>890 ± 19.3</t>
-  </si>
-  <si>
-    <t>0.976 ± 0.02</t>
-  </si>
-  <si>
     <t>1.54 ± 0.03</t>
   </si>
   <si>
     <t>9.41  ± 0.029</t>
   </si>
   <si>
-    <t>1730 ± 7.25</t>
-  </si>
-  <si>
-    <t>618 ± 10.8</t>
-  </si>
-  <si>
     <t>9.06  ± 0.070</t>
   </si>
   <si>
-    <t>1740 ± 4.84</t>
-  </si>
-  <si>
     <t>1830 ± 7.17</t>
   </si>
   <si>
-    <t>743 ± 17.5</t>
-  </si>
-  <si>
     <t>9.11  ± 0.058</t>
   </si>
   <si>
     <t>1830 ± 7.27</t>
   </si>
   <si>
-    <t>555 ± 7.85</t>
-  </si>
-  <si>
     <t>7.82 ± 0.007</t>
   </si>
   <si>
@@ -254,24 +230,12 @@
     <t>7.86 ± 0.006</t>
   </si>
   <si>
-    <t>1.33 ± 0.02</t>
-  </si>
-  <si>
-    <t>1.13 ± 0.02</t>
-  </si>
-  <si>
-    <t>1.43 ± 0.02</t>
-  </si>
-  <si>
     <t>2.1 ± 0.03</t>
   </si>
   <si>
     <t>1.79 ± 0.04</t>
   </si>
   <si>
-    <t>2.26 ± 0.04</t>
-  </si>
-  <si>
     <t>26.1 ± 0.13</t>
   </si>
   <si>
@@ -297,9 +261,6 @@
   </si>
   <si>
     <t>7.88 ± 0.005</t>
-  </si>
-  <si>
-    <t>1710 ± 6.40</t>
   </si>
   <si>
     <t>1830 ± 7.30</t>
@@ -330,7 +291,7 @@
   </si>
   <si>
     <r>
-      <t>(mol kgDW</t>
+      <t xml:space="preserve"> (µmol kgSW</t>
     </r>
     <r>
       <rPr>
@@ -354,7 +315,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve"> (µmol kgSW</t>
+      <t>(µmol kgSW</t>
     </r>
     <r>
       <rPr>
@@ -377,8 +338,50 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>(µmol kgSW</t>
+    <t xml:space="preserve">pH </t>
+  </si>
+  <si>
+    <t>2.25 ± 0.04</t>
+  </si>
+  <si>
+    <t>0.98 ± 0.02</t>
+  </si>
+  <si>
+    <t>1.32 ± 0.02</t>
+  </si>
+  <si>
+    <t>1.14 ± 0.02</t>
+  </si>
+  <si>
+    <t>1.42 ± 0.02</t>
+  </si>
+  <si>
+    <t>1770 ± 6.61</t>
+  </si>
+  <si>
+    <t>1730 ± 6.75</t>
+  </si>
+  <si>
+    <t>1740 ± 4.77</t>
+  </si>
+  <si>
+    <t>1710 ± 5.10</t>
+  </si>
+  <si>
+    <t>893 ± 18.9</t>
+  </si>
+  <si>
+    <t>616 ± 10.9</t>
+  </si>
+  <si>
+    <t>745 ± 17.6</t>
+  </si>
+  <si>
+    <t>553 ± 7.5</t>
+  </si>
+  <si>
+    <r>
+      <t>(mol kgSW</t>
     </r>
     <r>
       <rPr>
@@ -399,9 +402,6 @@
       </rPr>
       <t>)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">pH </t>
   </si>
 </sst>
 </file>
@@ -1321,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="P17" sqref="A1:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="12" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="M5" s="12" t="s">
         <v>16</v>
@@ -1446,20 +1446,20 @@
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="13" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="M6" s="13" t="s">
         <v>10</v>
@@ -1522,24 +1522,24 @@
       <c r="H9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>26</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="O9" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="N9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O9" s="14" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1551,11 +1551,11 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="14"/>
       <c r="K10" s="3"/>
       <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
+      <c r="M10" s="9"/>
       <c r="N10" s="14"/>
       <c r="O10" s="14"/>
     </row>
@@ -1571,35 +1571,35 @@
         <v>28</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1631,35 +1631,35 @@
         <v>29</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="9" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="M13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="O13" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="N13" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="O13" s="9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1691,35 +1691,35 @@
         <v>24</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="9" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="3" customHeight="1" x14ac:dyDescent="0.3">
@@ -1832,6 +1832,7 @@
       <c r="J23"/>
       <c r="K23"/>
       <c r="L23"/>
+      <c r="M23"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B24"/>
@@ -1845,18 +1846,100 @@
       <c r="J24"/>
       <c r="K24"/>
       <c r="L24"/>
+      <c r="M24"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I27" s="14"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I28" s="14"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I29" s="14"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I30" s="14"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I31" s="14"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I32" s="14"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I33" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>